<commit_message>
Change locations for NX stuff
</commit_message>
<xml_diff>
--- a/Template.xlsx
+++ b/Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lukie\source\repos\SimsigImporter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C540868E-D60B-440E-9170-E7D3D6A6BE11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B5EC37F-CDD5-4288-B336-9F5D1AB41F45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1161C59C-3AE7-4B35-ABC8-2123C8C6623B}"/>
+    <workbookView xWindow="19090" yWindow="-10830" windowWidth="38620" windowHeight="21220" activeTab="1" xr2:uid="{1161C59C-3AE7-4B35-ABC8-2123C8C6623B}"/>
   </bookViews>
   <sheets>
     <sheet name="Seed Groups" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="57">
   <si>
     <t>ID</t>
   </si>
@@ -210,6 +210,12 @@
   </si>
   <si>
     <t>INSERTHERE</t>
+  </si>
+  <si>
+    <t>1M00</t>
+  </si>
+  <si>
+    <t>1M01</t>
   </si>
 </sst>
 </file>
@@ -641,7 +647,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7858847A-F0D3-434C-9565-DB06C73D8860}">
   <dimension ref="A1:G1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
@@ -674,13 +680,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A52C7610-3C21-45C1-A819-83D8DB5DD38A}">
   <dimension ref="A1:I77"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" customWidth="1"/>
+    <col min="1" max="1" width="26.7109375" customWidth="1"/>
+    <col min="2" max="2" width="30.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -711,7 +718,9 @@
         <v>51</v>
       </c>
       <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
+      <c r="C4" s="4" t="s">
+        <v>55</v>
+      </c>
       <c r="D4" s="11"/>
       <c r="E4" s="11"/>
     </row>
@@ -1329,12 +1338,13 @@
   <dimension ref="A1:L77"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" customWidth="1"/>
+    <col min="1" max="1" width="27" customWidth="1"/>
+    <col min="2" max="2" width="25" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -1365,7 +1375,9 @@
         <v>51</v>
       </c>
       <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
+      <c r="C4" s="4" t="s">
+        <v>56</v>
+      </c>
       <c r="D4" s="11"/>
       <c r="E4" s="11"/>
     </row>

</xml_diff>